<commit_message>
Cambie cronograma post charla Lihuen
</commit_message>
<xml_diff>
--- a/Cronograma_MIDES.xlsx
+++ b/Cronograma_MIDES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alejandro\Research\MIDES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57C3677-C3E2-449C-A4F7-3D4CF8B51FD1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75004C54-712F-45FD-AF78-1E79F29D1BEE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{9CB1E32A-FCD9-40BD-85DB-33C002F60006}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Ene</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Matcheo de nuevos datos conseguidos en base MIDES</t>
+  </si>
+  <si>
+    <t>Ago</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -463,7 +466,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -493,15 +495,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,148 +822,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA0FC69-E998-4857-A018-809583FA17B9}">
-  <dimension ref="B1:AG27"/>
+  <dimension ref="B1:AK27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="68" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="33" width="3" style="1" customWidth="1"/>
-    <col min="34" max="34" width="4" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="37" width="3.140625" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22"/>
-      <c r="C2" s="31">
+    <row r="1" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="21"/>
+      <c r="C2" s="32">
         <v>2018</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
       <c r="F2" s="32">
         <v>2019</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="33"/>
-    </row>
-    <row r="3" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30"/>
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="31"/>
+    </row>
+    <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="31" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="31" t="s">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="31" t="s">
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="32" t="s">
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="W3" s="32"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="31" t="s">
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AA3" s="32"/>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="33"/>
-      <c r="AD3" s="32" t="s">
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AE3" s="32"/>
-      <c r="AF3" s="32"/>
-      <c r="AG3" s="33"/>
-    </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="AE3" s="30"/>
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI3" s="30"/>
+      <c r="AJ3" s="30"/>
+      <c r="AK3" s="31"/>
+    </row>
+    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="24"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
       <c r="AG4" s="25"/>
-    </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="AH4" s="33"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="35"/>
+    </row>
+    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="15"/>
@@ -990,10 +1011,14 @@
       <c r="AD5" s="4"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
-      <c r="AG5" s="6"/>
-    </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="6"/>
+    </row>
+    <row r="6" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="15"/>
@@ -1026,10 +1051,14 @@
       <c r="AD6" s="4"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
-      <c r="AG6" s="6"/>
-    </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="6"/>
+    </row>
+    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="15"/>
@@ -1062,10 +1091,14 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
-      <c r="AG7" s="6"/>
-    </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="6"/>
+    </row>
+    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="15"/>
@@ -1098,10 +1131,14 @@
       <c r="AD8" s="4"/>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
-      <c r="AG8" s="6"/>
-    </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="6"/>
+    </row>
+    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="15"/>
@@ -1134,10 +1171,14 @@
       <c r="AD9" s="4"/>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
-      <c r="AG9" s="6"/>
-    </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
+      <c r="AG9" s="11"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="6"/>
+    </row>
+    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="15"/>
@@ -1170,10 +1211,14 @@
       <c r="AD10" s="4"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
-      <c r="AG10" s="6"/>
-    </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="6"/>
+    </row>
+    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="15"/>
@@ -1206,10 +1251,14 @@
       <c r="AD11" s="4"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
-      <c r="AG11" s="6"/>
-    </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="6"/>
+    </row>
+    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="15"/>
@@ -1242,10 +1291,14 @@
       <c r="AD12" s="4"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
-      <c r="AG12" s="6"/>
-    </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="6"/>
+    </row>
+    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="15"/>
@@ -1278,10 +1331,14 @@
       <c r="AD13" s="4"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
-      <c r="AG13" s="6"/>
-    </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="6"/>
+    </row>
+    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="15"/>
@@ -1314,10 +1371,14 @@
       <c r="AD14" s="4"/>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
-      <c r="AG14" s="6"/>
-    </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="6"/>
+    </row>
+    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B15" s="19" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="15"/>
@@ -1350,10 +1411,14 @@
       <c r="AD15" s="4"/>
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
-      <c r="AG15" s="6"/>
-    </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="5"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="6"/>
+    </row>
+    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B16" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="5"/>
@@ -1386,10 +1451,14 @@
       <c r="AD16" s="4"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
-      <c r="AG16" s="6"/>
-    </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="6"/>
+    </row>
+    <row r="17" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="5"/>
@@ -1422,10 +1491,14 @@
       <c r="AD17" s="4"/>
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
-      <c r="AG17" s="6"/>
-    </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="6"/>
+    </row>
+    <row r="18" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B18" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="5"/>
@@ -1458,10 +1531,14 @@
       <c r="AD18" s="4"/>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
-      <c r="AG18" s="6"/>
-    </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="6"/>
+    </row>
+    <row r="19" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="5"/>
@@ -1473,12 +1550,12 @@
       <c r="I19" s="6"/>
       <c r="J19" s="5"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="7"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="6"/>
       <c r="N19" s="4"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="11"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="14"/>
       <c r="R19" s="5"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
@@ -1494,10 +1571,14 @@
       <c r="AD19" s="4"/>
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
-      <c r="AG19" s="6"/>
-    </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="6"/>
+    </row>
+    <row r="20" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="5"/>
@@ -1509,12 +1590,12 @@
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="7"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="6"/>
       <c r="N20" s="4"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="11"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="14"/>
       <c r="R20" s="5"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
@@ -1530,10 +1611,14 @@
       <c r="AD20" s="4"/>
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
-      <c r="AG20" s="6"/>
-    </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="AG20" s="11"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="2"/>
+      <c r="AK20" s="6"/>
+    </row>
+    <row r="21" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="5"/>
@@ -1545,12 +1630,12 @@
       <c r="I21" s="6"/>
       <c r="J21" s="5"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="7"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="6"/>
       <c r="N21" s="4"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="11"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="14"/>
       <c r="R21" s="5"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
@@ -1566,10 +1651,14 @@
       <c r="AD21" s="4"/>
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
-      <c r="AG21" s="6"/>
-    </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="5"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+      <c r="AK21" s="6"/>
+    </row>
+    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="5"/>
@@ -1578,15 +1667,15 @@
       <c r="F22" s="5"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="6"/>
       <c r="J22" s="15"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="11"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="14"/>
       <c r="R22" s="5"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
@@ -1602,10 +1691,14 @@
       <c r="AD22" s="4"/>
       <c r="AE22" s="2"/>
       <c r="AF22" s="2"/>
-      <c r="AG22" s="6"/>
-    </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="s">
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="6"/>
+    </row>
+    <row r="23" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="5"/>
@@ -1619,14 +1712,14 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="6"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="6"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="7"/>
       <c r="V23" s="4"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
@@ -1638,10 +1731,14 @@
       <c r="AD23" s="4"/>
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
-      <c r="AG23" s="6"/>
-    </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="5"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="6"/>
+    </row>
+    <row r="24" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B24" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="5"/>
@@ -1659,14 +1756,14 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="11"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="11"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="14"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
@@ -1674,10 +1771,14 @@
       <c r="AD24" s="4"/>
       <c r="AE24" s="2"/>
       <c r="AF24" s="2"/>
-      <c r="AG24" s="6"/>
-    </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
+      <c r="AG24" s="11"/>
+      <c r="AH24" s="5"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="6"/>
+    </row>
+    <row r="25" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="5"/>
@@ -1699,21 +1800,25 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="6"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="14"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="2"/>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="6"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="7"/>
       <c r="AD25" s="4"/>
       <c r="AE25" s="2"/>
       <c r="AF25" s="2"/>
-      <c r="AG25" s="6"/>
-    </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
+      <c r="AG25" s="11"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="6"/>
+    </row>
+    <row r="26" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="5"/>
@@ -1739,17 +1844,21 @@
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="11"/>
-      <c r="Z26" s="15"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="7"/>
-      <c r="AD26" s="4"/>
-      <c r="AE26" s="2"/>
-      <c r="AF26" s="2"/>
-      <c r="AG26" s="6"/>
-    </row>
-    <row r="27" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="21" t="s">
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="16"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="14"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="6"/>
+    </row>
+    <row r="27" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="8"/>
@@ -1779,15 +1888,20 @@
       <c r="AA27" s="9"/>
       <c r="AB27" s="9"/>
       <c r="AC27" s="10"/>
-      <c r="AD27" s="17"/>
-      <c r="AE27" s="18"/>
-      <c r="AF27" s="18"/>
-      <c r="AG27" s="19"/>
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="12"/>
+      <c r="AH27" s="36"/>
+      <c r="AI27" s="17"/>
+      <c r="AJ27" s="17"/>
+      <c r="AK27" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="F2:AK2"/>
     <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="F2:AG2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F3:I3"/>

</xml_diff>